<commit_message>
merge in main xls template
</commit_message>
<xml_diff>
--- a/tests/data/0311_Template_MAWebApp.xlsx
+++ b/tests/data/0311_Template_MAWebApp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/Desktop/Research/GloBI/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761CDD3-12C7-0541-A72A-D2EFB63557EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8F1DA-FBA0-6345-95E6-0D8EB0C32AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="22" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3145" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="857">
   <si>
     <t>Name</t>
   </si>
@@ -24358,9 +24358,9 @@
   </sheetPr>
   <dimension ref="A1:CF89"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25358,9 +25358,12 @@
       <c r="A15" t="s">
         <v>843</v>
       </c>
+      <c r="B15" t="s">
+        <v>268</v>
+      </c>
       <c r="C15" t="str">
         <f>IF(_xlfn.XLOOKUP(B15,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B15,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer and inner roofs of the building</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -25413,9 +25416,12 @@
       <c r="A16" t="s">
         <v>844</v>
       </c>
+      <c r="B16" t="s">
+        <v>268</v>
+      </c>
       <c r="C16" t="str">
         <f>IF(_xlfn.XLOOKUP(B16,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B16,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer and inner roofs of the building</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -25468,6 +25474,9 @@
       <c r="A17" t="s">
         <v>845</v>
       </c>
+      <c r="B17" t="s">
+        <v>268</v>
+      </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>[]</v>
@@ -25515,9 +25524,12 @@
       <c r="A18" t="s">
         <v>846</v>
       </c>
+      <c r="B18" t="s">
+        <v>270</v>
+      </c>
       <c r="C18" t="str">
         <f>IF(_xlfn.XLOOKUP(B17,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B17,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer and inner roofs of the building</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -25570,9 +25582,12 @@
       <c r="A19" t="s">
         <v>847</v>
       </c>
+      <c r="B19" t="s">
+        <v>270</v>
+      </c>
       <c r="C19" t="str">
         <f>IF(_xlfn.XLOOKUP(B18,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B18,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer walls/façade of the building</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -25625,9 +25640,12 @@
       <c r="A20" t="s">
         <v>848</v>
       </c>
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
       <c r="C20" t="str">
         <f>IF(_xlfn.XLOOKUP(B19,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B19,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer walls/façade of the building</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -25679,7 +25697,7 @@
     <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="C21" t="str">
         <f>IF(_xlfn.XLOOKUP(B20,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B20,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer walls/façade of the building</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -29016,7 +29034,7 @@
   <mergeCells count="1">
     <mergeCell ref="F1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:B83 R6:R83">
+  <conditionalFormatting sqref="R6:R83 A6:B83">
     <cfRule type="containsBlanks" dxfId="23" priority="9">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
@@ -29049,7 +29067,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B5B1DDB0-401F-D640-AA84-BB55E26336C9}">
           <x14:formula1>
             <xm:f>Drop_downs!$A$3:$A$9</xm:f>
@@ -29087,8 +29105,8 @@
   </sheetPr>
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30079,103 +30097,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.08</v>
+        <v>0.98</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.28999999999999998</v>
+        <v>0.64</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32</v>
+        <v>0.9</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.22</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.75</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.21</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78</v>
+        <v>0.71</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48</v>
+        <v>0.99</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23</v>
+        <v>0.81</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34</v>
+        <v>0.89</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.5</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26</v>
+        <v>0.09</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42</v>
+        <v>0.82</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.43</v>
+        <v>0.68</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98</v>
+        <v>0.34</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51</v>
+        <v>0.04</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.72</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61</v>
+        <v>0.46</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -36412,11 +36430,11 @@
         <v>Template_MA_SF_OLD</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:B3">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
+        <f t="array" ref="B2:B6">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
         <v>Template_MA_MF_NEW_roof</v>
       </c>
       <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2:C3">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
+        <f t="array" ref="C2:C6">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
         <v>TEMPLATE_MF_MA_LOW_facade</v>
       </c>
       <c r="D2" t="str" cm="1">
@@ -36454,16 +36472,34 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="str">
+        <v>Low_insulation_roof_MA_SFH</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Low_insulation_wall_MA_SFH</v>
+      </c>
       <c r="I4" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="str">
+        <v>Medium_insulation_roof_MA_SFH</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Med_insulation_wall_MA_SFH</v>
+      </c>
       <c r="I5" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="str">
+        <v>High_insulation_roof_MA_SFH</v>
+      </c>
+      <c r="C6" t="str">
+        <v>High_insulation_wall_MA_SFH</v>
+      </c>
       <c r="I6" t="s">
         <v>461</v>
       </c>

</xml_diff>

<commit_message>
merge in template from main
</commit_message>
<xml_diff>
--- a/tests/data/0311_Template_MAWebApp.xlsx
+++ b/tests/data/0311_Template_MAWebApp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/Desktop/Research/GloBI/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761CDD3-12C7-0541-A72A-D2EFB63557EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8F1DA-FBA0-6345-95E6-0D8EB0C32AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="22" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3145" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="857">
   <si>
     <t>Name</t>
   </si>
@@ -24358,9 +24358,9 @@
   </sheetPr>
   <dimension ref="A1:CF89"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25358,9 +25358,12 @@
       <c r="A15" t="s">
         <v>843</v>
       </c>
+      <c r="B15" t="s">
+        <v>268</v>
+      </c>
       <c r="C15" t="str">
         <f>IF(_xlfn.XLOOKUP(B15,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B15,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer and inner roofs of the building</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -25413,9 +25416,12 @@
       <c r="A16" t="s">
         <v>844</v>
       </c>
+      <c r="B16" t="s">
+        <v>268</v>
+      </c>
       <c r="C16" t="str">
         <f>IF(_xlfn.XLOOKUP(B16,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B16,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer and inner roofs of the building</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -25468,6 +25474,9 @@
       <c r="A17" t="s">
         <v>845</v>
       </c>
+      <c r="B17" t="s">
+        <v>268</v>
+      </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>[]</v>
@@ -25515,9 +25524,12 @@
       <c r="A18" t="s">
         <v>846</v>
       </c>
+      <c r="B18" t="s">
+        <v>270</v>
+      </c>
       <c r="C18" t="str">
         <f>IF(_xlfn.XLOOKUP(B17,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B17,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer and inner roofs of the building</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -25570,9 +25582,12 @@
       <c r="A19" t="s">
         <v>847</v>
       </c>
+      <c r="B19" t="s">
+        <v>270</v>
+      </c>
       <c r="C19" t="str">
         <f>IF(_xlfn.XLOOKUP(B18,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B18,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer walls/façade of the building</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -25625,9 +25640,12 @@
       <c r="A20" t="s">
         <v>848</v>
       </c>
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
       <c r="C20" t="str">
         <f>IF(_xlfn.XLOOKUP(B19,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B19,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer walls/façade of the building</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -25679,7 +25697,7 @@
     <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="C21" t="str">
         <f>IF(_xlfn.XLOOKUP(B20,Units!$A$2:$A$100,Units!$C$2:$C$100,"")=0,"Waiting for inputs in Column B",_xlfn.XLOOKUP(B20,Units!$A$2:$A$100,Units!$C$2:$C$100,""))</f>
-        <v>Waiting for inputs in Column B</v>
+        <v>Construction for the outer walls/façade of the building</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -29016,7 +29034,7 @@
   <mergeCells count="1">
     <mergeCell ref="F1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:B83 R6:R83">
+  <conditionalFormatting sqref="R6:R83 A6:B83">
     <cfRule type="containsBlanks" dxfId="23" priority="9">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
@@ -29049,7 +29067,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B5B1DDB0-401F-D640-AA84-BB55E26336C9}">
           <x14:formula1>
             <xm:f>Drop_downs!$A$3:$A$9</xm:f>
@@ -29087,8 +29105,8 @@
   </sheetPr>
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30079,103 +30097,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.08</v>
+        <v>0.98</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.28999999999999998</v>
+        <v>0.64</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32</v>
+        <v>0.9</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.22</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.75</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.21</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78</v>
+        <v>0.71</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48</v>
+        <v>0.99</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23</v>
+        <v>0.81</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34</v>
+        <v>0.89</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.5</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26</v>
+        <v>0.09</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42</v>
+        <v>0.82</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.43</v>
+        <v>0.68</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98</v>
+        <v>0.34</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51</v>
+        <v>0.04</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.72</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61</v>
+        <v>0.46</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -36412,11 +36430,11 @@
         <v>Template_MA_SF_OLD</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:B3">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
+        <f t="array" ref="B2:B6">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=B$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
         <v>Template_MA_MF_NEW_roof</v>
       </c>
       <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2:C3">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
+        <f t="array" ref="C2:C6">_xlfn._xlws.FILTER(IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,""),IF(Construction_components!$B:$B=C$1,Construction_components!$A:$A,"")&lt;&gt;"")</f>
         <v>TEMPLATE_MF_MA_LOW_facade</v>
       </c>
       <c r="D2" t="str" cm="1">
@@ -36454,16 +36472,34 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="str">
+        <v>Low_insulation_roof_MA_SFH</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Low_insulation_wall_MA_SFH</v>
+      </c>
       <c r="I4" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="str">
+        <v>Medium_insulation_roof_MA_SFH</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Med_insulation_wall_MA_SFH</v>
+      </c>
       <c r="I5" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="str">
+        <v>High_insulation_roof_MA_SFH</v>
+      </c>
+      <c r="C6" t="str">
+        <v>High_insulation_wall_MA_SFH</v>
+      </c>
       <c r="I6" t="s">
         <v>461</v>
       </c>

</xml_diff>